<commit_message>
Donation without test order class added
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/Drop2defects.xlsx
+++ b/BloodstreamAPI/testData/Drop2defects.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{94578ED6-E8B6-4426-89F5-6F36B9D709E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7766DC56-4FEE-4241-B4BB-BE4D8C3BEFCC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="5745" tabRatio="715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13740" windowHeight="9585" tabRatio="715" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidPaginationParam73560" sheetId="2" r:id="rId1"/>
     <sheet name="FlagnameSorting74472" sheetId="3" r:id="rId2"/>
     <sheet name="AssaySorting74979" sheetId="4" r:id="rId3"/>
     <sheet name="PoolDetail75101" sheetId="5" r:id="rId4"/>
-    <sheet name="StatusHistoryOrderWithoutTests7" sheetId="6" r:id="rId5"/>
+    <sheet name="StatusHistoryWithoutTests75017" sheetId="6" r:id="rId5"/>
     <sheet name="UnauthorizedUser75039" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I17"/>
+  <oleSize ref="A4:M26"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>PageSize</t>
   </si>
@@ -73,9 +74,6 @@
     <t>TestInfoInvalidPoolDetail</t>
   </si>
   <si>
-    <t>TestInfoBlankPoolDetail</t>
-  </si>
-  <si>
     <t>PoolID</t>
   </si>
   <si>
@@ -85,37 +83,46 @@
     <t>Assert200</t>
   </si>
   <si>
+    <t>Assert401</t>
+  </si>
+  <si>
+    <t>/donationInfo/orderTestStatusHistory</t>
+  </si>
+  <si>
+    <t>donationId</t>
+  </si>
+  <si>
+    <t>requestId</t>
+  </si>
+  <si>
+    <t>DEV104</t>
+  </si>
+  <si>
+    <t>DEV104-2020065</t>
+  </si>
+  <si>
+    <t>/donationInfo/orderTests</t>
+  </si>
+  <si>
+    <t>UnauthorizedAccess</t>
+  </si>
+  <si>
+    <t>JFH1</t>
+  </si>
+  <si>
+    <t>JFH1-2020079</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>abc44</t>
+  </si>
+  <si>
     <t>Assert404</t>
   </si>
   <si>
-    <t>Assert401</t>
-  </si>
-  <si>
-    <t>/donationInfo/orderTestStatusHistory</t>
-  </si>
-  <si>
-    <t>donationId</t>
-  </si>
-  <si>
-    <t>requestId</t>
-  </si>
-  <si>
-    <t>DEV104</t>
-  </si>
-  <si>
-    <t>DEV104-2020065</t>
-  </si>
-  <si>
-    <t>DEVa1</t>
-  </si>
-  <si>
-    <t>DEVa1-2020052</t>
-  </si>
-  <si>
-    <t>/donationInfo/orderTests</t>
-  </si>
-  <si>
-    <t>UnauthorizedAccess</t>
+    <t>ac1</t>
   </si>
 </sst>
 </file>
@@ -196,15 +203,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -491,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC16E1A-EBE8-4FD7-9522-847FD03243A9}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -506,13 +511,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -556,11 +561,11 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
@@ -584,11 +589,11 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -632,13 +637,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -682,13 +687,13 @@
       <c r="E4" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -744,13 +749,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -803,78 +808,43 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CFD1AC-F7EA-42BA-81BE-C2671A4EF4C3}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>4564564</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -883,70 +853,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7575DF3-D978-46D7-B155-5BBA7276C842}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -958,12 +930,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
@@ -972,24 +944,24 @@
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -1001,7 +973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -1015,16 +987,18 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
-      </c>
-    </row>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1033,26 +1007,26 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -1064,14 +1038,14 @@
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1081,4 +1055,18 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D617BEA5-AA35-4ED9-9319-FACA25E7B3CC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added many test cases from Drop 3 and done code changes.
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/Drop2defects.xlsx
+++ b/BloodstreamAPI/testData/Drop2defects.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7766DC56-4FEE-4241-B4BB-BE4D8C3BEFCC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{637954F7-A5FA-4FE3-B385-0F160E1FEB77}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13740" windowHeight="9585" tabRatio="715" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13740" windowHeight="9585" tabRatio="715" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidPaginationParam73560" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A4:M26"/>
+  <oleSize ref="A1:N28"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
   <si>
     <t>PageSize</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>ac1</t>
+  </si>
+  <si>
+    <t>Assays:ASC</t>
   </si>
 </sst>
 </file>
@@ -740,13 +743,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C86503-788D-4884-8809-D8E5123B042C}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
@@ -774,18 +781,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -798,6 +805,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
+    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
@@ -853,9 +861,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7575DF3-D978-46D7-B155-5BBA7276C842}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -902,9 +910,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -913,7 +919,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -930,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -947,7 +953,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
@@ -956,7 +962,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
@@ -973,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -990,7 +996,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A6:E6"/>

</xml_diff>